<commit_message>
finshed test cases in adding new cus
</commit_message>
<xml_diff>
--- a/Bug.xlsx
+++ b/Bug.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdulrahmanAyman\Desktop\Testing Tasks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mn\Documents\GitHub\Manual-Testing---Bank-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8BC3B6-E866-426B-99D0-D129354A521D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D814DB-AC60-4598-8FE3-4823DDD49896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Title</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Attachement</t>
+  </si>
+  <si>
+    <t>opening_bug</t>
+  </si>
+  <si>
+    <t>the bar is not working</t>
+  </si>
+  <si>
+    <t>the bar goes to the botom and the user cant see the website</t>
   </si>
 </sst>
 </file>
@@ -398,31 +407,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D79112-6971-4B71-B22E-60920B345156}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.08984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="29.36328125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="25.36328125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="30.6328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="28.90625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.36328125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="26.36328125" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="22.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -458,6 +467,17 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>